<commit_message>
fix bug of vietin
</commit_message>
<xml_diff>
--- a/adg-api/src/main/resources/viettin/bang-ke-chung-tu-dien-tu-de-nghi-giai-ngan.xlsx
+++ b/adg-api/src/main/resources/viettin/bang-ke-chung-tu-dien-tu-de-nghi-giai-ngan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luan.phm/engineering/Projects/ADongGroup/adg-services-v2/adg-api/src/main/resources/viettin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45BD8795-BD18-D54A-A979-799249B53306}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E518A8D-44BE-3F4A-A056-0B6C83B5D38C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34400" yWindow="460" windowWidth="34400" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -83,7 +83,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -94,39 +94,51 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="&quot;Times New Roman&quot;"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="&quot;Times New Roman&quot;"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <i/>
       <sz val="12"/>
       <color rgb="FF404040"/>
-      <name val="&quot;Times New Roman&quot;"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="13"/>
       <color theme="1"/>
-      <name val="&quot;Times New Roman&quot;"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <i/>
       <sz val="13"/>
       <color theme="1"/>
-      <name val="&quot;Times New Roman&quot;"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -190,49 +202,53 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -453,11 +469,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A3:F19"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="7.5" customWidth="1"/>
     <col min="3" max="3" width="14.6640625" customWidth="1"/>
@@ -465,129 +481,195 @@
     <col min="5" max="5" width="38.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:6" ht="15">
-      <c r="A3" s="8" t="s">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+      <c r="A3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="D3" s="8" t="s">
+      <c r="B3" s="10"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-    </row>
-    <row r="4" spans="1:6" ht="15">
-      <c r="A4" s="8" t="s">
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+    </row>
+    <row r="4" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+      <c r="A4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="D4" s="8" t="s">
+      <c r="B4" s="10"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-    </row>
-    <row r="5" spans="1:6" ht="15">
-      <c r="A5" s="8" t="s">
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+    </row>
+    <row r="5" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+      <c r="A5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="7"/>
-    </row>
-    <row r="8" spans="1:6" ht="15">
-      <c r="A8" s="8" t="s">
+      <c r="B5" s="10"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+      <c r="A8" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-    </row>
-    <row r="9" spans="1:6" ht="15">
-      <c r="A9" s="1" t="s">
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+    </row>
+    <row r="9" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+      <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="13">
-      <c r="A10" s="16"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-    </row>
-    <row r="11" spans="1:6" ht="15">
-      <c r="A11" s="3"/>
-      <c r="B11" s="9" t="s">
+    <row r="10" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A10" s="4"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+      <c r="A11" s="6"/>
+      <c r="B11" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-    </row>
-    <row r="13" spans="1:6" ht="15">
-      <c r="B13" s="11" t="s">
+      <c r="C11" s="13"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+      <c r="A13" s="1"/>
+      <c r="B13" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-    </row>
-    <row r="14" spans="1:6" ht="15">
-      <c r="B14" s="12" t="s">
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+    </row>
+    <row r="14" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+      <c r="A14" s="1"/>
+      <c r="B14" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-    </row>
-    <row r="15" spans="1:6" ht="14">
-      <c r="B15" s="13" t="s">
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+    </row>
+    <row r="15" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A15" s="1"/>
+      <c r="B15" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-    </row>
-    <row r="17" spans="4:6" ht="16">
-      <c r="D17" s="14" t="s">
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-    </row>
-    <row r="18" spans="4:6" ht="23.25" customHeight="1">
-      <c r="D18" s="15" t="s">
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+    </row>
+    <row r="18" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-    </row>
-    <row r="19" spans="4:6" ht="17">
-      <c r="D19" s="6" t="s">
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+    </row>
+    <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="13">

</xml_diff>